<commit_message>
Queries updated join sql queries for Tree and bubble chart.
</commit_message>
<xml_diff>
--- a/DB/sample/Pie-SiteDemandByWaterSource.xlsx
+++ b/DB/sample/Pie-SiteDemandByWaterSource.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\WegotProject\Report\WorkingDir\Report\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\WegotProject\Report\WorkingDir\Report\DB\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="821" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="INFO" sheetId="9" r:id="rId1"/>
-    <sheet name="w2_water_source_type" sheetId="1" r:id="rId2"/>
+    <sheet name="Request Info" sheetId="9" r:id="rId1"/>
+    <sheet name="Water Sources" sheetId="1" r:id="rId2"/>
     <sheet name="WTP" sheetId="6" r:id="rId3"/>
     <sheet name="Flush" sheetId="8" r:id="rId4"/>
     <sheet name="Domestic" sheetId="7" r:id="rId5"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -56,53 +56,240 @@
     <t>Flush</t>
   </si>
   <si>
-    <t>Site ID</t>
-  </si>
-  <si>
-    <t>From Date</t>
-  </si>
-  <si>
-    <t>To Date</t>
-  </si>
-  <si>
-    <t>Chart Type</t>
-  </si>
-  <si>
-    <t>Pie</t>
-  </si>
-  <si>
-    <t>Table Name</t>
-  </si>
-  <si>
-    <t>Available Data</t>
-  </si>
-  <si>
-    <t>w2_water_source_type</t>
-  </si>
-  <si>
-    <t>All Available water sources</t>
-  </si>
-  <si>
-    <t>SELECT component_id FROM prod_we2db.w2_wtp where site_id=4;</t>
-  </si>
-  <si>
     <t>ASE371700018</t>
   </si>
   <si>
     <t>ASE371700019</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>component_id</t>
+  </si>
+  <si>
+    <t>Ahad Euphoria</t>
+  </si>
+  <si>
+    <t>Pie Chart</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>chartType</t>
+  </si>
+  <si>
+    <t>QUERY</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>w2_water_source_type;</t>
+    </r>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>gate_id</t>
+  </si>
+  <si>
+    <t>wtp_id</t>
+  </si>
+  <si>
+    <t>WTP Component ID List</t>
+  </si>
+  <si>
+    <t>SELECT * FROM w2_wtp WHERE site_id=4;</t>
+  </si>
+  <si>
+    <t>WTP Component ID - 1</t>
+  </si>
+  <si>
+    <t>comp_id</t>
+  </si>
+  <si>
+    <t>wtp_cat</t>
+  </si>
+  <si>
+    <t>day_total</t>
+  </si>
+  <si>
+    <t>cum</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>AGA371700003</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">FROM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">w2_wtp_component_day_total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">WHERE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>wtp_id=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6897BB"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">AND </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(dt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>BETWEEN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> '2018-04-01 00:00:00' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> '2018-04-30 23:59:59' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +424,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFCC7832"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6897BB"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -419,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -534,6 +746,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -579,13 +806,41 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -911,57 +1166,48 @@
   <dimension ref="B2:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43109</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C2" s="5">
+        <v>43191</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43112</v>
-      </c>
-      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4</v>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -973,83 +1219,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A3:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1057,58 +1318,1282 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J6"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="127" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="K3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8">
+        <v>29</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>29</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="J9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>150</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>177200</v>
+      </c>
+      <c r="G11" s="14">
+        <v>11859700</v>
+      </c>
+      <c r="H11" s="15">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>151</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>182900</v>
+      </c>
+      <c r="G12" s="14">
+        <v>11837800</v>
+      </c>
+      <c r="H12" s="15">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>152</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>131500</v>
+      </c>
+      <c r="G13" s="14">
+        <v>11991300</v>
+      </c>
+      <c r="H13" s="15">
+        <v>43192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>153</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <v>135600</v>
+      </c>
+      <c r="G14" s="14">
+        <v>11973500</v>
+      </c>
+      <c r="H14" s="15">
+        <v>43192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>154</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>193000</v>
+      </c>
+      <c r="G15" s="14">
+        <v>12184400</v>
+      </c>
+      <c r="H15" s="15">
+        <v>43193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>155</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <v>197900</v>
+      </c>
+      <c r="G16" s="14">
+        <v>12171500</v>
+      </c>
+      <c r="H16" s="15">
+        <v>43193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>156</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="13">
+        <v>161100</v>
+      </c>
+      <c r="G17" s="14">
+        <v>12345600</v>
+      </c>
+      <c r="H17" s="15">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>157</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13">
+        <v>152000</v>
+      </c>
+      <c r="G18" s="14">
+        <v>12323600</v>
+      </c>
+      <c r="H18" s="15">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>158</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="13">
+        <v>164700</v>
+      </c>
+      <c r="G19" s="14">
+        <v>12510400</v>
+      </c>
+      <c r="H19" s="15">
+        <v>43195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>159</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13">
+        <v>168300</v>
+      </c>
+      <c r="G20" s="14">
+        <v>12492000</v>
+      </c>
+      <c r="H20" s="15">
+        <v>43195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>160</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="F21" s="13">
+        <v>196100</v>
+      </c>
+      <c r="G21" s="14">
+        <v>12706600</v>
+      </c>
+      <c r="H21" s="15">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>161</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="13">
+        <v>199800</v>
+      </c>
+      <c r="G22" s="14">
+        <v>12691900</v>
+      </c>
+      <c r="H22" s="15">
+        <v>43196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>162</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>165800</v>
+      </c>
+      <c r="G23" s="14">
+        <v>12872400</v>
+      </c>
+      <c r="H23" s="15">
+        <v>43197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>163</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13">
+        <v>168700</v>
+      </c>
+      <c r="G24" s="14">
+        <v>12860600</v>
+      </c>
+      <c r="H24" s="15">
+        <v>43197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>164</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13">
+        <v>128800</v>
+      </c>
+      <c r="G25" s="14">
+        <v>13001200</v>
+      </c>
+      <c r="H25" s="15">
+        <v>43198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>165</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13">
+        <v>132700</v>
+      </c>
+      <c r="G26" s="14">
+        <v>12993300</v>
+      </c>
+      <c r="H26" s="15">
+        <v>43198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>166</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13">
+        <v>149200</v>
+      </c>
+      <c r="G27" s="14">
+        <v>13142600</v>
+      </c>
+      <c r="H27" s="15">
+        <v>43199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>167</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
+      <c r="F28" s="13">
+        <v>145800</v>
+      </c>
+      <c r="G28" s="14">
+        <v>13147200</v>
+      </c>
+      <c r="H28" s="15">
+        <v>43199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>168</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8">
+        <v>1</v>
+      </c>
+      <c r="F29" s="13">
+        <v>129400</v>
+      </c>
+      <c r="G29" s="14">
+        <v>13311800</v>
+      </c>
+      <c r="H29" s="15">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>169</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="13">
+        <v>130900</v>
+      </c>
+      <c r="G30" s="14">
+        <v>13317400</v>
+      </c>
+      <c r="H30" s="15">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>170</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="13">
+        <v>174700</v>
+      </c>
+      <c r="G31" s="14">
+        <v>13492100</v>
+      </c>
+      <c r="H31" s="15">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>171</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13">
+        <v>161900</v>
+      </c>
+      <c r="G32" s="14">
+        <v>13473700</v>
+      </c>
+      <c r="H32" s="15">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>172</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="8">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
+      <c r="F33" s="13">
+        <v>147700</v>
+      </c>
+      <c r="G33" s="14">
+        <v>13621400</v>
+      </c>
+      <c r="H33" s="15">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>173</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+      <c r="F34" s="13">
+        <v>146300</v>
+      </c>
+      <c r="G34" s="14">
+        <v>13638400</v>
+      </c>
+      <c r="H34" s="15">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>174</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8">
+        <v>1</v>
+      </c>
+      <c r="F35" s="13">
+        <v>123700</v>
+      </c>
+      <c r="G35" s="14">
+        <v>13745200</v>
+      </c>
+      <c r="H35" s="15">
+        <v>43203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>175</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="8">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
+      <c r="F36" s="13">
+        <v>123000</v>
+      </c>
+      <c r="G36" s="14">
+        <v>13761500</v>
+      </c>
+      <c r="H36" s="15">
+        <v>43203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>176</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="8">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0</v>
+      </c>
+      <c r="F37" s="13">
+        <v>179700</v>
+      </c>
+      <c r="G37" s="14">
+        <v>13941300</v>
+      </c>
+      <c r="H37" s="15">
+        <v>43204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>177</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13">
+        <v>180500</v>
+      </c>
+      <c r="G38" s="14">
+        <v>13925900</v>
+      </c>
+      <c r="H38" s="15">
+        <v>43204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>178</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1</v>
+      </c>
+      <c r="E39" s="8">
+        <v>0</v>
+      </c>
+      <c r="F39" s="13">
+        <v>136100</v>
+      </c>
+      <c r="G39" s="14">
+        <v>14077500</v>
+      </c>
+      <c r="H39" s="15">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>179</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="8">
+        <v>1</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1</v>
+      </c>
+      <c r="F40" s="13">
+        <v>124700</v>
+      </c>
+      <c r="G40" s="14">
+        <v>14050700</v>
+      </c>
+      <c r="H40" s="15">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>180</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1</v>
+      </c>
+      <c r="E41" s="8">
+        <v>1</v>
+      </c>
+      <c r="F41" s="13">
+        <v>132000</v>
+      </c>
+      <c r="G41" s="14">
+        <v>14182900</v>
+      </c>
+      <c r="H41" s="15">
+        <v>43206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>181</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1</v>
+      </c>
+      <c r="E42" s="8">
+        <v>0</v>
+      </c>
+      <c r="F42" s="13">
+        <v>129400</v>
+      </c>
+      <c r="G42" s="14">
+        <v>14207100</v>
+      </c>
+      <c r="H42" s="15">
+        <v>43206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>182</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="8">
+        <v>1</v>
+      </c>
+      <c r="E43" s="8">
+        <v>1</v>
+      </c>
+      <c r="F43" s="13">
+        <v>142105</v>
+      </c>
+      <c r="G43" s="14">
+        <v>14325102</v>
+      </c>
+      <c r="H43" s="15">
+        <v>43207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>183</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="8">
+        <v>1</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0</v>
+      </c>
+      <c r="F44" s="13">
+        <v>143500</v>
+      </c>
+      <c r="G44" s="14">
+        <v>14350900</v>
+      </c>
+      <c r="H44" s="15">
+        <v>43207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>184</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="8">
+        <v>1</v>
+      </c>
+      <c r="E45" s="8">
+        <v>1</v>
+      </c>
+      <c r="F45" s="13">
+        <v>158498</v>
+      </c>
+      <c r="G45" s="14">
+        <v>14483697</v>
+      </c>
+      <c r="H45" s="15">
+        <v>43208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>185</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="8">
+        <v>1</v>
+      </c>
+      <c r="E46" s="8">
+        <v>0</v>
+      </c>
+      <c r="F46" s="13">
+        <v>161600</v>
+      </c>
+      <c r="G46" s="14">
+        <v>14512700</v>
+      </c>
+      <c r="H46" s="15">
+        <v>43208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>186</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="8">
+        <v>1</v>
+      </c>
+      <c r="E47" s="8">
+        <v>0</v>
+      </c>
+      <c r="F47" s="13">
+        <v>180500</v>
+      </c>
+      <c r="G47" s="14">
+        <v>14693500</v>
+      </c>
+      <c r="H47" s="15">
+        <v>43209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>187</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="8">
+        <v>1</v>
+      </c>
+      <c r="E48" s="8">
+        <v>1</v>
+      </c>
+      <c r="F48" s="13">
+        <v>178286</v>
+      </c>
+      <c r="G48" s="14">
+        <v>14662177</v>
+      </c>
+      <c r="H48" s="15">
+        <v>43209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>188</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="8">
+        <v>1</v>
+      </c>
+      <c r="E49" s="8">
+        <v>0</v>
+      </c>
+      <c r="F49" s="13">
+        <v>21400</v>
+      </c>
+      <c r="G49" s="14">
+        <v>14979600</v>
+      </c>
+      <c r="H49" s="15">
+        <v>43211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>189</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="8">
+        <v>1</v>
+      </c>
+      <c r="E50" s="8">
+        <v>1</v>
+      </c>
+      <c r="F50" s="13">
+        <v>21534</v>
+      </c>
+      <c r="G50" s="14">
+        <v>14946872</v>
+      </c>
+      <c r="H50" s="15">
+        <v>43211</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>190</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="8">
+        <v>1</v>
+      </c>
+      <c r="E51" s="8">
+        <v>1</v>
+      </c>
+      <c r="F51" s="13">
+        <v>120959</v>
+      </c>
+      <c r="G51" s="14">
+        <v>15067928</v>
+      </c>
+      <c r="H51" s="15">
+        <v>43212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>191</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="8">
+        <v>1</v>
+      </c>
+      <c r="E52" s="8">
+        <v>0</v>
+      </c>
+      <c r="F52" s="13">
+        <v>120900</v>
+      </c>
+      <c r="G52" s="14">
+        <v>15100600</v>
+      </c>
+      <c r="H52" s="15">
+        <v>43212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>192</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1</v>
+      </c>
+      <c r="E53" s="8">
+        <v>0</v>
+      </c>
+      <c r="F53" s="8">
+        <v>-100</v>
+      </c>
+      <c r="G53" s="14">
+        <v>15102000</v>
+      </c>
+      <c r="H53" s="15">
+        <v>43213</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:J2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>